<commit_message>
tested and working with simulation
</commit_message>
<xml_diff>
--- a/experiment/template/experiment_configurations.xlsx
+++ b/experiment/template/experiment_configurations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\stepped-dpu\incremental_changes\stepped-dpu\experiment\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\simulated-dpu\dpu\experiment\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD57FF7-77A2-4C28-B7FC-72FFF999CF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563AFA9E-F5D5-4EB5-85CD-B01EC1FB5AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{AF0A681E-4FC9-47B3-B0CB-C8A6E2C1048C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{AF0A681E-4FC9-47B3-B0CB-C8A6E2C1048C}"/>
   </bookViews>
   <sheets>
     <sheet name="selection-control" sheetId="3" r:id="rId1"/>
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A245ECA0-28EC-4A16-B4DE-14A4BDF7F5DD}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>40</v>
@@ -809,10 +809,10 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I2">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -847,10 +847,10 @@
         <v>6</v>
       </c>
       <c r="H3">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -867,7 +867,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -885,10 +885,10 @@
         <v>6</v>
       </c>
       <c r="H4">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -905,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -923,10 +923,10 @@
         <v>6</v>
       </c>
       <c r="H5">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -961,10 +961,10 @@
         <v>6</v>
       </c>
       <c r="H6">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -999,10 +999,10 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I7">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1037,10 +1037,10 @@
         <v>6</v>
       </c>
       <c r="H8">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I8">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -1075,10 +1075,10 @@
         <v>6</v>
       </c>
       <c r="H9">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I9">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -1113,10 +1113,10 @@
         <v>6</v>
       </c>
       <c r="H10">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I10">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -1151,10 +1151,10 @@
         <v>6</v>
       </c>
       <c r="H11">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I11">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -1189,10 +1189,10 @@
         <v>6</v>
       </c>
       <c r="H12">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I12">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J12">
         <v>2</v>
@@ -1227,10 +1227,10 @@
         <v>6</v>
       </c>
       <c r="H13">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I13">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1247,7 +1247,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -1265,10 +1265,10 @@
         <v>6</v>
       </c>
       <c r="H14">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I14">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -1285,7 +1285,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>40</v>
@@ -1303,10 +1303,10 @@
         <v>6</v>
       </c>
       <c r="H15">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I15">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -1323,7 +1323,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>40</v>
@@ -1341,10 +1341,10 @@
         <v>6</v>
       </c>
       <c r="H16">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1361,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>40</v>
@@ -1379,10 +1379,10 @@
         <v>6</v>
       </c>
       <c r="H17">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="I17">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1404,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49C5A42-5AA9-4484-8593-A550BEA149B1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1440,13 +1440,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1454,16 +1454,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1607,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1624,7 +1624,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1715,7 +1715,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1752,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1760,7 +1760,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1848,7 +1848,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1856,7 +1856,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle chemical vs non-chemical selection
</commit_message>
<xml_diff>
--- a/experiment/template/experiment_configurations.xlsx
+++ b/experiment/template/experiment_configurations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\simulated-dpu\dpu\experiment\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\stepped-dpu\stepped-dpu\experiment\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563AFA9E-F5D5-4EB5-85CD-B01EC1FB5AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C00584-76FD-4D69-B144-7F5E81CD5E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{AF0A681E-4FC9-47B3-B0CB-C8A6E2C1048C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{AF0A681E-4FC9-47B3-B0CB-C8A6E2C1048C}"/>
   </bookViews>
   <sheets>
     <sheet name="selection-control" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{63DEB4E8-EB73-439A-BC9B-98194E237881}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EE95CE7B-1B53-4764-B91A-3EA95F1200B3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>chemical: using a chemical selection. Slow pumps will be used to adjust chemical concentration
+non-chemical: anything that does not require fluidics</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{63DEB4E8-EB73-439A-BC9B-98194E237881}">
       <text>
         <r>
           <rPr>
@@ -69,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{66FAE453-068B-4933-A0A6-6A71E935D7C6}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{66FAE453-068B-4933-A0A6-6A71E935D7C6}">
       <text>
         <r>
           <rPr>
@@ -82,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{028F0605-8E5D-4C20-811E-5A2E01F240A4}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{028F0605-8E5D-4C20-811E-5A2E01F240A4}">
       <text>
         <r>
           <rPr>
@@ -95,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{E36F93DF-EBE8-44D1-AF93-062AA8622028}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E36F93DF-EBE8-44D1-AF93-062AA8622028}">
       <text>
         <r>
           <rPr>
@@ -108,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{7473487C-EAD0-4619-B744-412D2C5EC02E}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{7473487C-EAD0-4619-B744-412D2C5EC02E}">
       <text>
         <r>
           <rPr>
@@ -121,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2CBD995A-BE07-4274-980F-D6F88C704C98}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{2CBD995A-BE07-4274-980F-D6F88C704C98}">
       <text>
         <r>
           <rPr>
@@ -134,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{344A0881-BD8B-4858-8DEB-95058FAFC86E}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{344A0881-BD8B-4858-8DEB-95058FAFC86E}">
       <text>
         <r>
           <rPr>
@@ -148,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{CA271D26-FA8F-49F9-B5DB-55713FC402EB}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{CA271D26-FA8F-49F9-B5DB-55713FC402EB}">
       <text>
         <r>
           <rPr>
@@ -161,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{9BDA1110-A0F3-4860-AAF6-E4BC1B99B5CA}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{9BDA1110-A0F3-4860-AAF6-E4BC1B99B5CA}">
       <text>
         <r>
           <rPr>
@@ -265,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>vial</t>
   </si>
@@ -334,13 +348,22 @@
   </si>
   <si>
     <t>step_type</t>
+  </si>
+  <si>
+    <t>selection_type</t>
+  </si>
+  <si>
+    <t>chemical</t>
+  </si>
+  <si>
+    <t>non-chemical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +384,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -727,28 +756,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A245ECA0-28EC-4A16-B4DE-14A4BDF7F5DD}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.68359375" customWidth="1"/>
-    <col min="5" max="5" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.05078125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.20703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.20703125" customWidth="1"/>
+    <col min="4" max="4" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.68359375" customWidth="1"/>
+    <col min="6" max="6" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.05078125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.20703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,641 +786,692 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
         <v>40</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.1</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.12</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
         <v>40</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.12</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.5</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
         <v>40</v>
       </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
         <v>7</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.1</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.12</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
         <v>40</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>6</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.1</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.12</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.5</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
         <v>40</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>6</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.12</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.5</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
         <v>40</v>
       </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>6</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.1</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.12</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.5</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
         <v>40</v>
       </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.12</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.5</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
         <v>40</v>
       </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.12</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.5</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
         <v>40</v>
       </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>6</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.1</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.12</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>2</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.5</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
         <v>40</v>
       </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
         <v>7</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>6</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.1</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.12</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.5</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
         <v>40</v>
       </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
         <v>7</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>6</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.1</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.12</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.5</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
         <v>40</v>
       </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
       <c r="E13">
         <v>5</v>
       </c>
       <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
         <v>7</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>6</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.1</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.12</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.5</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
         <v>40</v>
       </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
         <v>7</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>6</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.1</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.12</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>2</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.5</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
         <v>40</v>
       </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
       <c r="E15">
         <v>5</v>
       </c>
       <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
         <v>7</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>6</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.1</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.12</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>2</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.5</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
         <v>40</v>
       </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
       <c r="E16">
         <v>5</v>
       </c>
       <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
         <v>7</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>6</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.1</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.12</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.5</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
         <v>40</v>
       </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
         <v>7</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>6</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.1</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.12</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.5</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1404,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49C5A42-5AA9-4484-8593-A550BEA149B1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Generalized SteppedController to diff types of selection
</commit_message>
<xml_diff>
--- a/experiment/template/experiment_configurations.xlsx
+++ b/experiment/template/experiment_configurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\stepped-dpu\stepped-dpu\experiment\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C00584-76FD-4D69-B144-7F5E81CD5E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C87213-E42B-499E-807D-271B00ABAF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{AF0A681E-4FC9-47B3-B0CB-C8A6E2C1048C}"/>
   </bookViews>
@@ -80,6 +80,19 @@
             <family val="2"/>
           </rPr>
           <t>stock concentrations for each vial; should be low enough that minimum selection level is possible given min_bolus_s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C70218A6-8950-4FAE-978C-AC447FD968C7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>number of growth curves required at start of experiment before beginning selection</t>
         </r>
       </text>
     </comment>
@@ -279,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
   <si>
     <t>vial</t>
   </si>
@@ -354,9 +367,6 @@
   </si>
   <si>
     <t>chemical</t>
-  </si>
-  <si>
-    <t>non-chemical</t>
   </si>
 </sst>
 </file>
@@ -759,7 +769,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -827,7 +837,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -839,16 +849,16 @@
         <v>5</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J2">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -880,16 +890,16 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J3">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -921,16 +931,16 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J4">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -962,16 +972,16 @@
         <v>5</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J5">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K5">
         <v>2</v>
@@ -1003,16 +1013,16 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J6">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -1044,16 +1054,16 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J7">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -1085,16 +1095,16 @@
         <v>5</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J8">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1126,16 +1136,16 @@
         <v>5</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J9">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1167,16 +1177,16 @@
         <v>5</v>
       </c>
       <c r="G10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J10">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -1208,16 +1218,16 @@
         <v>5</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J11">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -1249,16 +1259,16 @@
         <v>5</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J12">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K12">
         <v>2</v>
@@ -1290,16 +1300,16 @@
         <v>5</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J13">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -1331,16 +1341,16 @@
         <v>5</v>
       </c>
       <c r="G14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J14">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K14">
         <v>2</v>
@@ -1372,16 +1382,16 @@
         <v>5</v>
       </c>
       <c r="G15">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J15">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K15">
         <v>2</v>
@@ -1413,16 +1423,16 @@
         <v>5</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J16">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -1454,16 +1464,16 @@
         <v>5</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J17">
-        <v>0.12</v>
+        <v>0.4</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -1486,7 +1496,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1541,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>20</v>

</xml_diff>